<commit_message>
Issue repaired regarding the use of float and integer when creating df_lca_lifespan
</commit_message>
<xml_diff>
--- a/BEM_LCA_Hypothesis.xlsx
+++ b/BEM_LCA_Hypothesis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0F7505-E499-4585-8AC0-24006C173D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D56118-A6C7-40D2-8FCC-B45AA4A62F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="930" windowWidth="28770" windowHeight="15270" tabRatio="822" firstSheet="9" activeTab="14" xr2:uid="{65AFDB44-F0B5-471D-BCAC-A3541777CAD5}"/>
+    <workbookView xWindow="30" yWindow="390" windowWidth="28770" windowHeight="15270" tabRatio="822" firstSheet="9" activeTab="11" xr2:uid="{65AFDB44-F0B5-471D-BCAC-A3541777CAD5}"/>
   </bookViews>
   <sheets>
     <sheet name="INTRO" sheetId="25" r:id="rId1"/>
@@ -4089,6 +4089,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4124,9 +4127,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5269,10 +5269,10 @@
       <c r="D4" s="11"/>
     </row>
     <row r="6" spans="2:23">
-      <c r="B6" s="241" t="s">
+      <c r="B6" s="242" t="s">
         <v>968</v>
       </c>
-      <c r="C6" s="241"/>
+      <c r="C6" s="242"/>
       <c r="D6" s="35"/>
       <c r="E6" s="28"/>
       <c r="F6" s="20"/>
@@ -5285,10 +5285,10 @@
       <c r="I6" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="S6" s="241" t="s">
+      <c r="S6" s="242" t="s">
         <v>523</v>
       </c>
-      <c r="T6" s="241"/>
+      <c r="T6" s="242"/>
       <c r="U6" s="35"/>
       <c r="V6" s="28"/>
       <c r="W6" s="99"/>
@@ -6919,10 +6919,10 @@
       <c r="B140" s="39"/>
     </row>
     <row r="141" spans="2:9">
-      <c r="B141" s="241" t="s">
+      <c r="B141" s="242" t="s">
         <v>387</v>
       </c>
-      <c r="C141" s="241"/>
+      <c r="C141" s="242"/>
       <c r="D141" s="35"/>
       <c r="E141" s="28"/>
       <c r="F141" s="20"/>
@@ -7324,10 +7324,10 @@
       </c>
     </row>
     <row r="179" spans="2:9">
-      <c r="B179" s="241" t="s">
+      <c r="B179" s="242" t="s">
         <v>388</v>
       </c>
-      <c r="C179" s="241"/>
+      <c r="C179" s="242"/>
       <c r="D179" s="35"/>
       <c r="E179" s="28"/>
       <c r="F179" s="20"/>
@@ -7614,10 +7614,10 @@
       </c>
     </row>
     <row r="206" spans="2:9">
-      <c r="B206" s="241" t="s">
+      <c r="B206" s="242" t="s">
         <v>981</v>
       </c>
-      <c r="C206" s="241"/>
+      <c r="C206" s="242"/>
       <c r="D206" s="35"/>
       <c r="E206" s="28"/>
       <c r="F206" s="237"/>
@@ -7885,7 +7885,7 @@
   <dimension ref="B1:W227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7928,10 +7928,10 @@
       <c r="D4" s="11"/>
     </row>
     <row r="6" spans="2:23">
-      <c r="B6" s="241" t="s">
+      <c r="B6" s="242" t="s">
         <v>1012</v>
       </c>
-      <c r="C6" s="241"/>
+      <c r="C6" s="242"/>
       <c r="D6" s="35"/>
       <c r="E6" s="28"/>
       <c r="F6" s="220"/>
@@ -7944,10 +7944,10 @@
       <c r="I6" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="S6" s="241" t="s">
+      <c r="S6" s="242" t="s">
         <v>523</v>
       </c>
-      <c r="T6" s="241"/>
+      <c r="T6" s="242"/>
       <c r="U6" s="35"/>
       <c r="V6" s="28"/>
       <c r="W6" s="220"/>
@@ -11045,10 +11045,10 @@
       <c r="B153" s="39"/>
     </row>
     <row r="154" spans="2:23">
-      <c r="B154" s="241" t="s">
+      <c r="B154" s="242" t="s">
         <v>387</v>
       </c>
-      <c r="C154" s="241"/>
+      <c r="C154" s="242"/>
       <c r="D154" s="35"/>
       <c r="E154" s="28"/>
       <c r="F154" s="220"/>
@@ -11355,10 +11355,10 @@
       </c>
     </row>
     <row r="181" spans="2:9">
-      <c r="B181" s="241" t="s">
+      <c r="B181" s="242" t="s">
         <v>388</v>
       </c>
-      <c r="C181" s="241"/>
+      <c r="C181" s="242"/>
       <c r="D181" s="35"/>
       <c r="E181" s="28"/>
       <c r="F181" s="220"/>
@@ -11645,10 +11645,10 @@
       </c>
     </row>
     <row r="207" spans="2:9">
-      <c r="B207" s="241" t="s">
+      <c r="B207" s="242" t="s">
         <v>981</v>
       </c>
-      <c r="C207" s="241"/>
+      <c r="C207" s="242"/>
       <c r="D207" s="35"/>
       <c r="E207" s="28"/>
       <c r="F207" s="237"/>
@@ -11915,8 +11915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CC6CCE-31D8-423C-980F-A2F1E6B19115}">
   <dimension ref="B1:W114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11959,10 +11959,10 @@
       <c r="D4" s="11"/>
     </row>
     <row r="6" spans="2:23">
-      <c r="B6" s="241" t="s">
+      <c r="B6" s="242" t="s">
         <v>642</v>
       </c>
-      <c r="C6" s="241"/>
+      <c r="C6" s="242"/>
       <c r="D6" s="35"/>
       <c r="E6" s="28"/>
       <c r="F6" s="128"/>
@@ -11975,10 +11975,10 @@
       <c r="I6" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="S6" s="241" t="s">
+      <c r="S6" s="242" t="s">
         <v>523</v>
       </c>
-      <c r="T6" s="241"/>
+      <c r="T6" s="242"/>
       <c r="U6" s="35"/>
       <c r="V6" s="28"/>
       <c r="W6" s="128"/>
@@ -13863,10 +13863,10 @@
       <c r="F3" s="41"/>
     </row>
     <row r="4" spans="2:6" s="11" customFormat="1">
-      <c r="B4" s="249" t="s">
+      <c r="B4" s="250" t="s">
         <v>390</v>
       </c>
-      <c r="C4" s="249"/>
+      <c r="C4" s="250"/>
       <c r="D4" s="35"/>
       <c r="E4" s="28"/>
       <c r="F4" s="20"/>
@@ -13956,10 +13956,10 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="249" t="s">
+      <c r="B15" s="250" t="s">
         <v>399</v>
       </c>
-      <c r="C15" s="249"/>
+      <c r="C15" s="250"/>
       <c r="D15" s="35"/>
       <c r="E15" s="28"/>
       <c r="F15" s="20"/>
@@ -14256,7 +14256,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A2:Q208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G174" sqref="G174"/>
     </sheetView>
   </sheetViews>
@@ -14281,17 +14281,17 @@
       <c r="F2" s="144"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="253" t="s">
         <v>612</v>
       </c>
-      <c r="B3" s="252"/>
-      <c r="C3" s="252"/>
-      <c r="D3" s="252"/>
-      <c r="E3" s="252"/>
-      <c r="F3" s="252"/>
-      <c r="G3" s="252"/>
-      <c r="H3" s="252"/>
-      <c r="I3" s="252"/>
+      <c r="B3" s="253"/>
+      <c r="C3" s="253"/>
+      <c r="D3" s="253"/>
+      <c r="E3" s="253"/>
+      <c r="F3" s="253"/>
+      <c r="G3" s="253"/>
+      <c r="H3" s="253"/>
+      <c r="I3" s="253"/>
       <c r="L3" s="139"/>
       <c r="M3" s="139"/>
     </row>
@@ -14603,7 +14603,7 @@
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
       <c r="A22" s="147"/>
-      <c r="B22" s="250" t="s">
+      <c r="B22" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C22" s="138" t="s">
@@ -14621,7 +14621,7 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
       <c r="A23" s="147"/>
-      <c r="B23" s="250"/>
+      <c r="B23" s="251"/>
       <c r="C23" s="136" t="s">
         <v>700</v>
       </c>
@@ -14637,7 +14637,7 @@
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
       <c r="A24" s="147"/>
-      <c r="B24" s="250"/>
+      <c r="B24" s="251"/>
       <c r="C24" s="136" t="s">
         <v>701</v>
       </c>
@@ -14655,7 +14655,7 @@
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
       <c r="A25" s="147"/>
-      <c r="B25" s="250"/>
+      <c r="B25" s="251"/>
       <c r="C25" s="136" t="s">
         <v>702</v>
       </c>
@@ -14671,7 +14671,7 @@
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
       <c r="A26" s="147"/>
-      <c r="B26" s="250"/>
+      <c r="B26" s="251"/>
       <c r="C26" s="136" t="s">
         <v>703</v>
       </c>
@@ -14687,7 +14687,7 @@
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1">
       <c r="A27" s="147"/>
-      <c r="B27" s="250"/>
+      <c r="B27" s="251"/>
       <c r="C27" s="136" t="s">
         <v>704</v>
       </c>
@@ -14701,7 +14701,7 @@
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1">
       <c r="A28" s="147"/>
-      <c r="B28" s="251"/>
+      <c r="B28" s="252"/>
       <c r="C28" s="137" t="s">
         <v>705</v>
       </c>
@@ -14729,17 +14729,17 @@
       <c r="K30" s="144"/>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1">
-      <c r="A31" s="252" t="s">
+      <c r="A31" s="253" t="s">
         <v>595</v>
       </c>
-      <c r="B31" s="252"/>
-      <c r="C31" s="252"/>
-      <c r="D31" s="252"/>
-      <c r="E31" s="252"/>
-      <c r="F31" s="252"/>
-      <c r="G31" s="252"/>
-      <c r="H31" s="252"/>
-      <c r="I31" s="252"/>
+      <c r="B31" s="253"/>
+      <c r="C31" s="253"/>
+      <c r="D31" s="253"/>
+      <c r="E31" s="253"/>
+      <c r="F31" s="253"/>
+      <c r="G31" s="253"/>
+      <c r="H31" s="253"/>
+      <c r="I31" s="253"/>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1">
       <c r="A32" s="139"/>
@@ -15014,7 +15014,7 @@
     </row>
     <row r="49" spans="1:15" ht="15" customHeight="1">
       <c r="A49" s="147"/>
-      <c r="B49" s="250" t="s">
+      <c r="B49" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C49" s="138" t="s">
@@ -15032,7 +15032,7 @@
     </row>
     <row r="50" spans="1:15" ht="15" customHeight="1">
       <c r="A50" s="147"/>
-      <c r="B50" s="250"/>
+      <c r="B50" s="251"/>
       <c r="C50" s="136" t="s">
         <v>700</v>
       </c>
@@ -15048,7 +15048,7 @@
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1">
       <c r="A51" s="147"/>
-      <c r="B51" s="250"/>
+      <c r="B51" s="251"/>
       <c r="C51" s="136" t="s">
         <v>701</v>
       </c>
@@ -15066,7 +15066,7 @@
     </row>
     <row r="52" spans="1:15" ht="15" customHeight="1">
       <c r="A52" s="147"/>
-      <c r="B52" s="250"/>
+      <c r="B52" s="251"/>
       <c r="C52" s="136" t="s">
         <v>702</v>
       </c>
@@ -15082,7 +15082,7 @@
     </row>
     <row r="53" spans="1:15" ht="15" customHeight="1">
       <c r="A53" s="147"/>
-      <c r="B53" s="250"/>
+      <c r="B53" s="251"/>
       <c r="C53" s="136" t="s">
         <v>703</v>
       </c>
@@ -15098,7 +15098,7 @@
     </row>
     <row r="54" spans="1:15" ht="15" customHeight="1">
       <c r="A54" s="147"/>
-      <c r="B54" s="250"/>
+      <c r="B54" s="251"/>
       <c r="C54" s="136" t="s">
         <v>704</v>
       </c>
@@ -15112,7 +15112,7 @@
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1">
       <c r="A55" s="147"/>
-      <c r="B55" s="251"/>
+      <c r="B55" s="252"/>
       <c r="C55" s="137" t="s">
         <v>705</v>
       </c>
@@ -15141,17 +15141,17 @@
       <c r="I57" s="139"/>
     </row>
     <row r="58" spans="1:15" ht="15" customHeight="1">
-      <c r="A58" s="252" t="s">
+      <c r="A58" s="253" t="s">
         <v>638</v>
       </c>
-      <c r="B58" s="252"/>
-      <c r="C58" s="252"/>
-      <c r="D58" s="252"/>
-      <c r="E58" s="252"/>
-      <c r="F58" s="252"/>
-      <c r="G58" s="252"/>
-      <c r="H58" s="252"/>
-      <c r="I58" s="252"/>
+      <c r="B58" s="253"/>
+      <c r="C58" s="253"/>
+      <c r="D58" s="253"/>
+      <c r="E58" s="253"/>
+      <c r="F58" s="253"/>
+      <c r="G58" s="253"/>
+      <c r="H58" s="253"/>
+      <c r="I58" s="253"/>
       <c r="L58" s="139"/>
       <c r="M58" s="139"/>
     </row>
@@ -15423,7 +15423,7 @@
     </row>
     <row r="77" spans="1:15" ht="15" customHeight="1">
       <c r="A77" s="147"/>
-      <c r="B77" s="250" t="s">
+      <c r="B77" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C77" s="140" t="s">
@@ -15441,7 +15441,7 @@
     </row>
     <row r="78" spans="1:15" ht="15" customHeight="1">
       <c r="A78" s="147"/>
-      <c r="B78" s="250"/>
+      <c r="B78" s="251"/>
       <c r="C78" s="170" t="s">
         <v>700</v>
       </c>
@@ -15457,7 +15457,7 @@
     </row>
     <row r="79" spans="1:15" ht="15" customHeight="1">
       <c r="A79" s="147"/>
-      <c r="B79" s="250"/>
+      <c r="B79" s="251"/>
       <c r="C79" s="170" t="s">
         <v>701</v>
       </c>
@@ -15475,7 +15475,7 @@
     </row>
     <row r="80" spans="1:15" ht="15" customHeight="1">
       <c r="A80" s="147"/>
-      <c r="B80" s="250"/>
+      <c r="B80" s="251"/>
       <c r="C80" s="170" t="s">
         <v>706</v>
       </c>
@@ -15491,7 +15491,7 @@
     </row>
     <row r="81" spans="1:15" ht="15" customHeight="1">
       <c r="A81" s="147"/>
-      <c r="B81" s="251"/>
+      <c r="B81" s="252"/>
       <c r="C81" s="171" t="s">
         <v>707</v>
       </c>
@@ -15525,17 +15525,17 @@
       <c r="K83" s="144"/>
     </row>
     <row r="84" spans="1:15" ht="15" customHeight="1">
-      <c r="A84" s="252" t="s">
+      <c r="A84" s="253" t="s">
         <v>613</v>
       </c>
-      <c r="B84" s="252"/>
-      <c r="C84" s="252"/>
-      <c r="D84" s="252"/>
-      <c r="E84" s="252"/>
-      <c r="F84" s="252"/>
-      <c r="G84" s="252"/>
-      <c r="H84" s="252"/>
-      <c r="I84" s="252"/>
+      <c r="B84" s="253"/>
+      <c r="C84" s="253"/>
+      <c r="D84" s="253"/>
+      <c r="E84" s="253"/>
+      <c r="F84" s="253"/>
+      <c r="G84" s="253"/>
+      <c r="H84" s="253"/>
+      <c r="I84" s="253"/>
       <c r="L84" s="139"/>
       <c r="M84" s="139"/>
     </row>
@@ -15899,17 +15899,17 @@
       <c r="K104" s="144"/>
     </row>
     <row r="105" spans="1:15" ht="15" customHeight="1">
-      <c r="A105" s="252" t="s">
+      <c r="A105" s="253" t="s">
         <v>593</v>
       </c>
-      <c r="B105" s="252"/>
-      <c r="C105" s="252"/>
-      <c r="D105" s="252"/>
-      <c r="E105" s="252"/>
-      <c r="F105" s="252"/>
-      <c r="G105" s="252"/>
-      <c r="H105" s="252"/>
-      <c r="I105" s="252"/>
+      <c r="B105" s="253"/>
+      <c r="C105" s="253"/>
+      <c r="D105" s="253"/>
+      <c r="E105" s="253"/>
+      <c r="F105" s="253"/>
+      <c r="G105" s="253"/>
+      <c r="H105" s="253"/>
+      <c r="I105" s="253"/>
     </row>
     <row r="106" spans="1:15" ht="15" customHeight="1">
       <c r="A106" s="147"/>
@@ -16133,7 +16133,7 @@
     </row>
     <row r="123" spans="1:7" ht="15" customHeight="1">
       <c r="A123" s="147"/>
-      <c r="B123" s="250" t="s">
+      <c r="B123" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C123" s="144" t="s">
@@ -16146,7 +16146,7 @@
     </row>
     <row r="124" spans="1:7" ht="15" customHeight="1">
       <c r="A124" s="147"/>
-      <c r="B124" s="250"/>
+      <c r="B124" s="251"/>
       <c r="C124" s="170" t="s">
         <v>700</v>
       </c>
@@ -16157,7 +16157,7 @@
     </row>
     <row r="125" spans="1:7" ht="15" customHeight="1">
       <c r="A125" s="147"/>
-      <c r="B125" s="250"/>
+      <c r="B125" s="251"/>
       <c r="C125" s="170" t="s">
         <v>701</v>
       </c>
@@ -16168,7 +16168,7 @@
     </row>
     <row r="126" spans="1:7" ht="15" customHeight="1">
       <c r="A126" s="147"/>
-      <c r="B126" s="250"/>
+      <c r="B126" s="251"/>
       <c r="C126" s="170" t="s">
         <v>706</v>
       </c>
@@ -16179,7 +16179,7 @@
     </row>
     <row r="127" spans="1:7" ht="15" customHeight="1">
       <c r="A127" s="147"/>
-      <c r="B127" s="251"/>
+      <c r="B127" s="252"/>
       <c r="C127" s="171" t="s">
         <v>707</v>
       </c>
@@ -16205,17 +16205,17 @@
       <c r="G129" s="139"/>
     </row>
     <row r="130" spans="1:15" ht="15" customHeight="1">
-      <c r="A130" s="252" t="s">
+      <c r="A130" s="253" t="s">
         <v>604</v>
       </c>
-      <c r="B130" s="252"/>
-      <c r="C130" s="252"/>
-      <c r="D130" s="252"/>
-      <c r="E130" s="252"/>
-      <c r="F130" s="252"/>
-      <c r="G130" s="252"/>
-      <c r="H130" s="252"/>
-      <c r="I130" s="252"/>
+      <c r="B130" s="253"/>
+      <c r="C130" s="253"/>
+      <c r="D130" s="253"/>
+      <c r="E130" s="253"/>
+      <c r="F130" s="253"/>
+      <c r="G130" s="253"/>
+      <c r="H130" s="253"/>
+      <c r="I130" s="253"/>
     </row>
     <row r="131" spans="1:15" ht="15" customHeight="1">
       <c r="A131" s="139"/>
@@ -16448,7 +16448,7 @@
     </row>
     <row r="148" spans="1:9" ht="15" customHeight="1">
       <c r="A148" s="139"/>
-      <c r="B148" s="250" t="s">
+      <c r="B148" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C148" s="144" t="s">
@@ -16460,7 +16460,7 @@
     </row>
     <row r="149" spans="1:9" ht="15" customHeight="1">
       <c r="A149" s="139"/>
-      <c r="B149" s="250"/>
+      <c r="B149" s="251"/>
       <c r="C149" s="170" t="s">
         <v>700</v>
       </c>
@@ -16470,7 +16470,7 @@
     </row>
     <row r="150" spans="1:9" ht="15" customHeight="1">
       <c r="A150" s="139"/>
-      <c r="B150" s="250"/>
+      <c r="B150" s="251"/>
       <c r="C150" s="170" t="s">
         <v>701</v>
       </c>
@@ -16483,7 +16483,7 @@
     </row>
     <row r="151" spans="1:9" ht="15" customHeight="1">
       <c r="A151" s="139"/>
-      <c r="B151" s="250"/>
+      <c r="B151" s="251"/>
       <c r="C151" s="170" t="s">
         <v>706</v>
       </c>
@@ -16496,7 +16496,7 @@
     </row>
     <row r="152" spans="1:9" ht="15" customHeight="1">
       <c r="A152" s="139"/>
-      <c r="B152" s="251"/>
+      <c r="B152" s="252"/>
       <c r="C152" s="171" t="s">
         <v>707</v>
       </c>
@@ -16528,17 +16528,17 @@
       <c r="I154" s="139"/>
     </row>
     <row r="155" spans="1:9" ht="15" customHeight="1">
-      <c r="A155" s="252" t="s">
+      <c r="A155" s="253" t="s">
         <v>635</v>
       </c>
-      <c r="B155" s="252"/>
-      <c r="C155" s="252"/>
-      <c r="D155" s="252"/>
-      <c r="E155" s="252"/>
-      <c r="F155" s="252"/>
-      <c r="G155" s="252"/>
-      <c r="H155" s="252"/>
-      <c r="I155" s="252"/>
+      <c r="B155" s="253"/>
+      <c r="C155" s="253"/>
+      <c r="D155" s="253"/>
+      <c r="E155" s="253"/>
+      <c r="F155" s="253"/>
+      <c r="G155" s="253"/>
+      <c r="H155" s="253"/>
+      <c r="I155" s="253"/>
     </row>
     <row r="156" spans="1:9" ht="15" customHeight="1">
       <c r="A156" s="139"/>
@@ -16814,7 +16814,7 @@
     </row>
     <row r="173" spans="1:15" ht="15" customHeight="1">
       <c r="A173" s="139"/>
-      <c r="B173" s="250" t="s">
+      <c r="B173" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C173" s="144" t="s">
@@ -16826,7 +16826,7 @@
     </row>
     <row r="174" spans="1:15" ht="15" customHeight="1">
       <c r="A174" s="139"/>
-      <c r="B174" s="250"/>
+      <c r="B174" s="251"/>
       <c r="C174" s="170" t="s">
         <v>700</v>
       </c>
@@ -16836,7 +16836,7 @@
     </row>
     <row r="175" spans="1:15" ht="15" customHeight="1">
       <c r="A175" s="139"/>
-      <c r="B175" s="250"/>
+      <c r="B175" s="251"/>
       <c r="C175" s="170" t="s">
         <v>701</v>
       </c>
@@ -16849,7 +16849,7 @@
     </row>
     <row r="176" spans="1:15" ht="15" customHeight="1">
       <c r="A176" s="139"/>
-      <c r="B176" s="250"/>
+      <c r="B176" s="251"/>
       <c r="C176" s="170" t="s">
         <v>706</v>
       </c>
@@ -16862,7 +16862,7 @@
     </row>
     <row r="177" spans="1:17" ht="15" customHeight="1">
       <c r="A177" s="139"/>
-      <c r="B177" s="251"/>
+      <c r="B177" s="252"/>
       <c r="C177" s="171" t="s">
         <v>707</v>
       </c>
@@ -16894,17 +16894,17 @@
       <c r="I179" s="139"/>
     </row>
     <row r="180" spans="1:17" ht="15" customHeight="1">
-      <c r="A180" s="252" t="s">
+      <c r="A180" s="253" t="s">
         <v>611</v>
       </c>
-      <c r="B180" s="252"/>
-      <c r="C180" s="252"/>
-      <c r="D180" s="252"/>
-      <c r="E180" s="252"/>
-      <c r="F180" s="252"/>
-      <c r="G180" s="252"/>
-      <c r="H180" s="252"/>
-      <c r="I180" s="252"/>
+      <c r="B180" s="253"/>
+      <c r="C180" s="253"/>
+      <c r="D180" s="253"/>
+      <c r="E180" s="253"/>
+      <c r="F180" s="253"/>
+      <c r="G180" s="253"/>
+      <c r="H180" s="253"/>
+      <c r="I180" s="253"/>
     </row>
     <row r="181" spans="1:17" ht="15" customHeight="1">
       <c r="A181" s="176" t="s">
@@ -16954,7 +16954,7 @@
       <c r="G183" s="143" t="s">
         <v>1042</v>
       </c>
-      <c r="H183" s="253" t="s">
+      <c r="H183" s="241" t="s">
         <v>536</v>
       </c>
       <c r="J183" s="146"/>
@@ -17205,7 +17205,7 @@
     </row>
     <row r="198" spans="1:15" ht="15" customHeight="1">
       <c r="A198" s="139"/>
-      <c r="B198" s="250" t="s">
+      <c r="B198" s="251" t="s">
         <v>601</v>
       </c>
       <c r="C198" s="144" t="s">
@@ -17220,7 +17220,7 @@
     </row>
     <row r="199" spans="1:15" ht="15" customHeight="1">
       <c r="A199" s="139"/>
-      <c r="B199" s="250"/>
+      <c r="B199" s="251"/>
       <c r="C199" s="170" t="s">
         <v>700</v>
       </c>
@@ -17233,7 +17233,7 @@
     </row>
     <row r="200" spans="1:15" ht="15" customHeight="1">
       <c r="A200" s="139"/>
-      <c r="B200" s="250"/>
+      <c r="B200" s="251"/>
       <c r="C200" s="170" t="s">
         <v>701</v>
       </c>
@@ -17246,7 +17246,7 @@
     </row>
     <row r="201" spans="1:15" ht="15" customHeight="1">
       <c r="A201" s="139"/>
-      <c r="B201" s="250"/>
+      <c r="B201" s="251"/>
       <c r="C201" s="170" t="s">
         <v>706</v>
       </c>
@@ -17259,7 +17259,7 @@
     </row>
     <row r="202" spans="1:15" ht="15" customHeight="1">
       <c r="A202" s="139"/>
-      <c r="B202" s="251"/>
+      <c r="B202" s="252"/>
       <c r="C202" s="171" t="s">
         <v>707</v>
       </c>
@@ -17310,6 +17310,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B198:B202"/>
+    <mergeCell ref="B173:B177"/>
+    <mergeCell ref="B148:B152"/>
+    <mergeCell ref="A105:I105"/>
+    <mergeCell ref="A130:I130"/>
+    <mergeCell ref="A155:I155"/>
+    <mergeCell ref="A180:I180"/>
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="B22:B28"/>
     <mergeCell ref="B123:B127"/>
@@ -17318,13 +17325,6 @@
     <mergeCell ref="A84:I84"/>
     <mergeCell ref="B49:B55"/>
     <mergeCell ref="A31:I31"/>
-    <mergeCell ref="B198:B202"/>
-    <mergeCell ref="B173:B177"/>
-    <mergeCell ref="B148:B152"/>
-    <mergeCell ref="A105:I105"/>
-    <mergeCell ref="A130:I130"/>
-    <mergeCell ref="A155:I155"/>
-    <mergeCell ref="A180:I180"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19083,10 +19083,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="242" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="241"/>
+      <c r="C4" s="242"/>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="11" t="s">
@@ -19097,10 +19097,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="241" t="s">
+      <c r="B8" s="242" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="241"/>
+      <c r="C8" s="242"/>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" s="11" t="s">
@@ -19125,10 +19125,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="17"/>
-      <c r="B16" s="242" t="s">
+      <c r="B16" s="243" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="242"/>
+      <c r="C16" s="243"/>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="11" t="s">
@@ -19136,10 +19136,10 @@
       </c>
     </row>
     <row r="20" spans="2:3" ht="138" customHeight="1">
-      <c r="B20" s="243" t="s">
+      <c r="B20" s="244" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="243"/>
+      <c r="C20" s="244"/>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="18" t="s">
@@ -19215,10 +19215,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="17"/>
-      <c r="B33" s="242" t="s">
+      <c r="B33" s="243" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="242"/>
+      <c r="C33" s="243"/>
     </row>
     <row r="34" spans="1:3">
       <c r="C34" s="16" t="s">
@@ -28516,10 +28516,10 @@
     </row>
     <row r="2" spans="2:6" s="11" customFormat="1"/>
     <row r="3" spans="2:6" s="11" customFormat="1">
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="242" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="241"/>
+      <c r="C3" s="242"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
@@ -28540,10 +28540,10 @@
     </row>
     <row r="5" spans="2:6" s="11" customFormat="1"/>
     <row r="6" spans="2:6" s="11" customFormat="1">
-      <c r="B6" s="241" t="s">
+      <c r="B6" s="242" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="241"/>
+      <c r="C6" s="242"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
@@ -28567,10 +28567,10 @@
     </row>
     <row r="8" spans="2:6" s="11" customFormat="1"/>
     <row r="9" spans="2:6" s="11" customFormat="1">
-      <c r="B9" s="241" t="s">
+      <c r="B9" s="242" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="241"/>
+      <c r="C9" s="242"/>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
@@ -29446,7 +29446,7 @@
       </c>
     </row>
     <row r="89" spans="2:5">
-      <c r="B89" s="243" t="s">
+      <c r="B89" s="244" t="s">
         <v>159</v>
       </c>
       <c r="C89" t="s">
@@ -29460,7 +29460,7 @@
       </c>
     </row>
     <row r="90" spans="2:5">
-      <c r="B90" s="243"/>
+      <c r="B90" s="244"/>
       <c r="C90" t="s">
         <v>147</v>
       </c>
@@ -29472,7 +29472,7 @@
       </c>
     </row>
     <row r="91" spans="2:5">
-      <c r="B91" s="243"/>
+      <c r="B91" s="244"/>
       <c r="C91" t="s">
         <v>148</v>
       </c>
@@ -29484,7 +29484,7 @@
       </c>
     </row>
     <row r="92" spans="2:5">
-      <c r="B92" s="243"/>
+      <c r="B92" s="244"/>
       <c r="C92" t="s">
         <v>149</v>
       </c>
@@ -31791,13 +31791,13 @@
       </c>
     </row>
     <row r="4" spans="1:32">
-      <c r="B4" s="246" t="s">
+      <c r="B4" s="247" t="s">
         <v>498</v>
       </c>
-      <c r="C4" s="246" t="s">
+      <c r="C4" s="247" t="s">
         <v>848</v>
       </c>
-      <c r="D4" s="246"/>
+      <c r="D4" s="247"/>
       <c r="E4" s="103" t="s">
         <v>449</v>
       </c>
@@ -31807,10 +31807,10 @@
       <c r="G4" s="103" t="s">
         <v>481</v>
       </c>
-      <c r="H4" s="244" t="s">
+      <c r="H4" s="245" t="s">
         <v>499</v>
       </c>
-      <c r="I4" s="244" t="s">
+      <c r="I4" s="245" t="s">
         <v>500</v>
       </c>
       <c r="J4"/>
@@ -31842,7 +31842,7 @@
       <c r="A5" s="134" t="s">
         <v>554</v>
       </c>
-      <c r="B5" s="247"/>
+      <c r="B5" s="248"/>
       <c r="C5" s="177" t="s">
         <v>419</v>
       </c>
@@ -31858,8 +31858,8 @@
       <c r="G5" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="245"/>
-      <c r="I5" s="245"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="246"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -36463,10 +36463,10 @@
       <c r="E3" s="26"/>
     </row>
     <row r="4" spans="2:12" s="11" customFormat="1">
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="242" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="241"/>
+      <c r="C4" s="242"/>
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -36566,10 +36566,10 @@
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="241" t="s">
+      <c r="B15" s="242" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="241"/>
+      <c r="C15" s="242"/>
       <c r="D15" s="27"/>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
@@ -36592,7 +36592,7 @@
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="248" t="s">
+      <c r="B17" s="249" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
@@ -36609,7 +36609,7 @@
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="248"/>
+      <c r="B18" s="249"/>
       <c r="C18" t="s">
         <v>211</v>
       </c>
@@ -36621,7 +36621,7 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="248"/>
+      <c r="B19" s="249"/>
       <c r="C19" t="s">
         <v>212</v>
       </c>
@@ -36783,10 +36783,10 @@
       </c>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="241" t="s">
+      <c r="B36" s="242" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="241"/>
+      <c r="C36" s="242"/>
       <c r="D36" s="27"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
@@ -37033,10 +37033,10 @@
       </c>
     </row>
     <row r="62" spans="2:6">
-      <c r="B62" s="241" t="s">
+      <c r="B62" s="242" t="s">
         <v>224</v>
       </c>
-      <c r="C62" s="241"/>
+      <c r="C62" s="242"/>
       <c r="D62" s="27"/>
       <c r="E62" s="28"/>
       <c r="F62" s="28"/>
@@ -37136,10 +37136,10 @@
       <c r="E3" s="26"/>
     </row>
     <row r="4" spans="2:6" s="11" customFormat="1">
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="242" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="241"/>
+      <c r="C4" s="242"/>
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -37209,10 +37209,10 @@
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="241" t="s">
+      <c r="B14" s="242" t="s">
         <v>942</v>
       </c>
-      <c r="C14" s="241"/>
+      <c r="C14" s="242"/>
       <c r="D14" s="27"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
@@ -37276,10 +37276,10 @@
       <c r="E3" s="26"/>
     </row>
     <row r="4" spans="2:6" s="11" customFormat="1">
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="242" t="s">
         <v>239</v>
       </c>
-      <c r="C4" s="241"/>
+      <c r="C4" s="242"/>
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -37355,10 +37355,10 @@
       <c r="E2" s="26"/>
     </row>
     <row r="3" spans="2:6" s="11" customFormat="1">
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="242" t="s">
         <v>427</v>
       </c>
-      <c r="C3" s="241"/>
+      <c r="C3" s="242"/>
       <c r="D3" s="35"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -37497,10 +37497,10 @@
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="241" t="s">
+      <c r="B20" s="242" t="s">
         <v>429</v>
       </c>
-      <c r="C20" s="241"/>
+      <c r="C20" s="242"/>
       <c r="D20" s="35" t="s">
         <v>419</v>
       </c>

</xml_diff>